<commit_message>
[SPIDERDROPPER] Improved PCB cradle.
</commit_message>
<xml_diff>
--- a/spider_dropper/spider_dropper_parts.xlsx
+++ b/spider_dropper/spider_dropper_parts.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\PrintableParts\spider_dropper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAC8E10-C73D-470A-9FD1-87603769CFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3760FBD6-AF1B-4C03-B12E-700CBD206AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="789" yWindow="1269" windowWidth="19851" windowHeight="15711" activeTab="1" xr2:uid="{92CA6418-27FC-4AD5-98BD-397EC845101D}"/>
+    <workbookView xWindow="789" yWindow="1269" windowWidth="19851" windowHeight="15711" xr2:uid="{92CA6418-27FC-4AD5-98BD-397EC845101D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Parts" sheetId="1" r:id="rId1"/>
+    <sheet name="Switches" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
   <si>
     <t>Spider Dropper Parts</t>
   </si>
@@ -88,9 +88,6 @@
     <t>AC Option</t>
   </si>
   <si>
-    <t>Common Parts</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -233,6 +230,87 @@
   </si>
   <si>
     <t>4. DigiKey claims it's no longer manufactured.</t>
+  </si>
+  <si>
+    <t>Slightly Smarter</t>
+  </si>
+  <si>
+    <t>Mechanical Parts</t>
+  </si>
+  <si>
+    <t>Slightly Smarter Electronics</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>https://www.pcbway.com/orderonline.aspx</t>
+  </si>
+  <si>
+    <t>PTC resettable fuse</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bel-fuse-inc/0ZRC0010FF1E/1560183</t>
+  </si>
+  <si>
+    <t>power connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/same-sky-formerly-cui-devices/PJ-102AH/408448</t>
+  </si>
+  <si>
+    <t>screw terminal</t>
+  </si>
+  <si>
+    <t>2N3904 NPN transistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/central-semiconductor-corp/2N3904-PBFREE/4806876</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/same-sky-formerly-cui-devices/TB007-508-02BE/10064127</t>
+  </si>
+  <si>
+    <t>TIP 120 Darlington transistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/TIP120/603564</t>
+  </si>
+  <si>
+    <t>resistors</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CFR-25JB-52-330R/1636</t>
+  </si>
+  <si>
+    <t>ZX-series microswitch</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/honeywell-sensing-and-productivity-solutions/ZX40E30C01/2748598</t>
+  </si>
+  <si>
+    <t>pin header sockets</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adam-tech/SMC-1-03-1-GT/9830940</t>
+  </si>
+  <si>
+    <t>1N4001 diode</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diotec-semiconductor/1N4001/13164614</t>
+  </si>
+  <si>
+    <t>HC-SR312 mini PIR</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B08PVB7VHQ/</t>
+  </si>
+  <si>
+    <t>DigiKey shipping is unpredictable and simply omitted.</t>
+  </si>
+  <si>
+    <t>Amazon shipping is free with Prime.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +378,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +386,7 @@
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -624,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49C792C-E920-409F-B110-1A72354C03E4}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -636,10 +715,11 @@
     <col min="11" max="11" width="2.921875" customWidth="1"/>
     <col min="12" max="12" width="10.69140625" customWidth="1"/>
     <col min="13" max="13" width="10.3828125" customWidth="1"/>
-    <col min="14" max="14" width="51.69140625" customWidth="1"/>
+    <col min="14" max="14" width="14.15234375" customWidth="1"/>
+    <col min="15" max="15" width="51.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -649,25 +729,28 @@
       <c r="M1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="N1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2</v>
@@ -679,14 +762,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
         <v>11.99</v>
@@ -695,7 +778,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1">
         <f>B4*0.1075</f>
@@ -717,13 +800,13 @@
         <f>H4*I4</f>
         <v>3.3197312500000002</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
         <v>11.99</v>
@@ -732,7 +815,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E8" si="0">B5*0.1075</f>
@@ -754,13 +837,13 @@
         <f>H5*I5</f>
         <v>0.88526166666666672</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>7.19</v>
@@ -769,7 +852,7 @@
         <v>330</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
@@ -791,16 +874,16 @@
         <f>H6*I6</f>
         <v>0.12065037878787879</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
@@ -823,9 +906,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1">
         <f>2*35.99</f>
@@ -835,7 +918,7 @@
         <v>2000</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -851,19 +934,19 @@
         <v>3.9858924999999996E-2</v>
       </c>
       <c r="I8">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" ref="J8" si="3">H8*I8</f>
-        <v>2.7104068999999997</v>
-      </c>
-      <c r="N8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+        <v>2.7901247499999999</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -875,129 +958,132 @@
       <c r="I9" s="3"/>
       <c r="J9" s="4">
         <f>SUM(J4:J8)</f>
-        <v>7.0360501954545454</v>
+        <v>7.115768045454546</v>
       </c>
       <c r="L9" s="1">
         <f>J9</f>
-        <v>7.0360501954545454</v>
+        <v>7.115768045454546</v>
       </c>
       <c r="M9" s="1">
         <f>J9</f>
-        <v>7.0360501954545454</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+        <v>7.115768045454546</v>
+      </c>
+      <c r="N9" s="1">
+        <f>J9</f>
+        <v>7.115768045454546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
-        <v>11.99</v>
+        <v>18.95</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
       <c r="E12" s="1">
-        <f t="shared" ref="E12:E14" si="4">B12*0.1075</f>
-        <v>1.2889250000000001</v>
-      </c>
-      <c r="F12" s="1"/>
+        <f t="shared" ref="E12:E13" si="4">B12*0.1075</f>
+        <v>2.0371250000000001</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9.5500000000000007</v>
+      </c>
       <c r="G12" s="1">
-        <f t="shared" ref="G12:G14" si="5">B12+E12+F12</f>
-        <v>13.278925000000001</v>
+        <f>B12+E12+F12</f>
+        <v>30.537125</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" ref="H12:H14" si="6">IF(C12&gt;0, G12/C12, 0)</f>
-        <v>13.278925000000001</v>
+        <f>IF(C12&gt;0, G12/C12, 0)</f>
+        <v>30.537125</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" s="1">
         <f>H12*I12</f>
-        <v>13.278925000000001</v>
-      </c>
-      <c r="N12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+        <v>30.537125</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>9.49</v>
+        <v>7.98</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="4"/>
-        <v>1.0201750000000001</v>
+        <v>0.85785</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
-        <f t="shared" si="5"/>
-        <v>10.510175</v>
+        <f t="shared" ref="G13" si="5">B13+E13+F13</f>
+        <v>8.8378499999999995</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="6"/>
-        <v>1.0510174999999999</v>
+        <f>IF(C13&gt;0, G13/C13, 0)</f>
+        <v>8.8378499999999999E-2</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J13" s="1">
         <f>H13*I13</f>
-        <v>1.0510174999999999</v>
-      </c>
-      <c r="N13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1">
-        <v>5.99</v>
-      </c>
-      <c r="C14">
-        <v>50</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="4"/>
-        <v>0.64392499999999997</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1">
-        <f t="shared" si="5"/>
-        <v>6.6339250000000005</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="6"/>
-        <v>0.1326785</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
-      </c>
-      <c r="J14" s="1">
-        <f>H14*I14</f>
-        <v>0.66339250000000005</v>
-      </c>
-      <c r="N14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>0.35351399999999999</v>
+      </c>
+      <c r="O13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4">
+        <f>SUM(J12:J13)</f>
+        <v>30.890639</v>
+      </c>
+      <c r="L14" s="1">
+        <f>J14</f>
+        <v>30.890639</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1006,107 +1092,128 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="4">
-        <f>SUM(J12:J14)</f>
-        <v>14.993335000000002</v>
-      </c>
-      <c r="M15" s="1">
-        <f>J15</f>
-        <v>14.993335000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="J15" s="4"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11.99</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" ref="E17:E19" si="6">B17*0.1075</f>
+        <v>1.2889250000000001</v>
+      </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="G17" s="1">
+        <f t="shared" ref="G17:G19" si="7">B17+E17+F17</f>
+        <v>13.278925000000001</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" ref="H17:H19" si="8">IF(C17&gt;0, G17/C17, 0)</f>
+        <v>13.278925000000001</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <f>H17*I17</f>
+        <v>13.278925000000001</v>
+      </c>
+      <c r="O17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>18.95</v>
+        <v>9.49</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18:E19" si="7">B18*0.1075</f>
-        <v>2.0371250000000001</v>
-      </c>
-      <c r="F18" s="1">
-        <v>9.5500000000000007</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>1.0201750000000001</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
-        <f>B18+E18+F18</f>
-        <v>30.537125</v>
+        <f t="shared" si="7"/>
+        <v>10.510175</v>
       </c>
       <c r="H18" s="1">
-        <f>IF(C18&gt;0, G18/C18, 0)</f>
-        <v>30.537125</v>
+        <f t="shared" si="8"/>
+        <v>1.0510174999999999</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" s="1">
         <f>H18*I18</f>
-        <v>30.537125</v>
-      </c>
-      <c r="N18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+        <v>1.0510174999999999</v>
+      </c>
+      <c r="O18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>7.98</v>
+        <v>5.99</v>
       </c>
       <c r="C19">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="7"/>
-        <v>0.85785</v>
+        <f t="shared" si="6"/>
+        <v>0.64392499999999997</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
-        <f t="shared" ref="G19" si="8">B19+E19+F19</f>
-        <v>8.8378499999999995</v>
+        <f t="shared" si="7"/>
+        <v>6.6339250000000005</v>
       </c>
       <c r="H19" s="1">
-        <f>IF(C19&gt;0, G19/C19, 0)</f>
-        <v>8.8378499999999999E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.1326785</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J19" s="1">
         <f>H19*I19</f>
-        <v>0.35351399999999999</v>
-      </c>
-      <c r="N19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+        <v>1.061428</v>
+      </c>
+      <c r="O19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1117,79 +1224,549 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="4">
-        <f>SUM(J18:J19)</f>
-        <v>30.890639</v>
-      </c>
-      <c r="L20" s="1">
+        <f>SUM(J17:J19)</f>
+        <v>15.391370500000001</v>
+      </c>
+      <c r="M20" s="1">
         <f>J20</f>
-        <v>30.890639</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="4" t="s">
+        <v>15.391370500000001</v>
+      </c>
+      <c r="N20" s="1">
+        <f>J20</f>
+        <v>15.391370500000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <v>19.98</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" ref="G23:G26" si="9">B23+E23+F23</f>
+        <v>24.98</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:H26" si="10">IF(C23&gt;0, G23/C23, 0)</f>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <f>H23*I23</f>
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="O23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" ref="E24" si="11">B24*0.1075</f>
+        <v>1.718925</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1">
+        <f t="shared" ref="G24" si="12">B24+E24+F24</f>
+        <v>17.708925000000001</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" ref="H24" si="13">IF(C24&gt;0, G24/C24, 0)</f>
+        <v>1.7708925</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <f>H24*I24</f>
+        <v>1.7708925</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.14</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" ref="E25:E26" si="14">B25*0.1075</f>
+        <v>0.23005</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
+        <f t="shared" si="9"/>
+        <v>2.37005</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="10"/>
+        <v>0.23700499999999999</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <f>H25*I25</f>
+        <v>0.23700499999999999</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="14"/>
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
+        <f t="shared" si="9"/>
+        <v>6.8665000000000003</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="10"/>
+        <v>0.68664999999999998</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <f>H26*I26</f>
+        <v>0.68664999999999998</v>
+      </c>
+      <c r="O26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.01</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" ref="E27" si="15">B27*0.1075</f>
+        <v>0.43107499999999999</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
+        <f t="shared" ref="G27" si="16">B27+E27+F27</f>
+        <v>4.4410749999999997</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27" si="17">IF(C27&gt;0, G27/C27, 0)</f>
+        <v>0.44410749999999999</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <f>H27*I27</f>
+        <v>0.44410749999999999</v>
+      </c>
+      <c r="O27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" ref="E28" si="18">B28*0.1075</f>
+        <v>0.17737499999999998</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1">
+        <f t="shared" ref="G28" si="19">B28+E28+F28</f>
+        <v>1.827375</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" ref="H28" si="20">IF(C28&gt;0, G28/C28, 0)</f>
+        <v>0.1827375</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <f>H28*I28</f>
+        <v>0.1827375</v>
+      </c>
+      <c r="O28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2.83</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" ref="E29" si="21">B29*0.1075</f>
+        <v>0.30422500000000002</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1">
+        <f t="shared" ref="G29" si="22">B29+E29+F29</f>
+        <v>3.1342250000000003</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" ref="H29" si="23">IF(C29&gt;0, G29/C29, 0)</f>
+        <v>0.31342250000000005</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <f>H29*I29</f>
+        <v>0.31342250000000005</v>
+      </c>
+      <c r="O29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1">
+        <v>27.04</v>
+      </c>
+      <c r="C30">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" ref="E30" si="24">B30*0.1075</f>
+        <v>2.9068000000000001</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1">
+        <f t="shared" ref="G30" si="25">B30+E30+F30</f>
+        <v>29.9468</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" ref="H30" si="26">IF(C30&gt;0, G30/C30, 0)</f>
+        <v>0.59893600000000002</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <f>H30*I30</f>
+        <v>0.59893600000000002</v>
+      </c>
+      <c r="O30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="C31">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" ref="E31:E32" si="27">B31*0.1075</f>
+        <v>0.14297500000000002</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1">
+        <f t="shared" ref="G31:G32" si="28">B31+E31+F31</f>
+        <v>1.4729750000000001</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" ref="H31:H32" si="29">IF(C31&gt;0, G31/C31, 0)</f>
+        <v>2.9459500000000003E-2</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1">
+        <f>H31*I31</f>
+        <v>5.8919000000000006E-2</v>
+      </c>
+      <c r="O31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="27"/>
+        <v>5.9125000000000004E-2</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1">
+        <f t="shared" si="28"/>
+        <v>0.60912500000000003</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="29"/>
+        <v>6.0912500000000001E-2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1">
+        <f>H32*I32</f>
+        <v>6.0912500000000001E-2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" ref="E33" si="30">B33*0.1075</f>
+        <v>0.53642500000000004</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1">
+        <f t="shared" ref="G33" si="31">B33+E33+F33</f>
+        <v>5.5264250000000006</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" ref="H33" si="32">IF(C33&gt;0, G33/C33, 0)</f>
+        <v>0.27632125000000002</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <f>H33*I33</f>
+        <v>0.27632125000000002</v>
+      </c>
+      <c r="O33" t="s">
+        <v>53</v>
+      </c>
+      <c r="P33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="4">
-        <f>SUM(L3:L21)</f>
-        <v>37.926689195454543</v>
-      </c>
-      <c r="M22" s="4">
-        <f>SUM(M3:M21)</f>
-        <v>22.029385195454548</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A28" s="5"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="4">
+        <f>SUM(J23:J33)</f>
+        <v>7.1279037499999998</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1">
+        <f>J34</f>
+        <v>7.1279037499999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="4">
+        <f>SUM(L3:L35)</f>
+        <v>38.006407045454544</v>
+      </c>
+      <c r="M36" s="4">
+        <f>SUM(M3:M35)</f>
+        <v>22.507138545454545</v>
+      </c>
+      <c r="N36" s="4">
+        <f>SUM(N3:N35)</f>
+        <v>29.635042295454546</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O24" r:id="rId1" xr:uid="{394BA01E-496A-4B9E-AF12-01E77921BE0E}"/>
+    <hyperlink ref="O25" r:id="rId2" xr:uid="{229E0547-4398-43AE-9042-0D4FDFFB3BD5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1197,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DF09C8-D9EA-4A94-8F05-63315EF27164}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1212,40 +1789,40 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1">
         <v>1.95</v>
@@ -1256,23 +1833,23 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1280,10 +1857,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="1">
         <v>1.75</v>
@@ -1291,30 +1868,30 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>1.33</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1">
         <v>0.25</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1">
         <v>2.31</v>
@@ -1325,32 +1902,32 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>